<commit_message>
starting simulation for only peak concentration
</commit_message>
<xml_diff>
--- a/Dx_1998_Li_et_al_2_Paper02_Chattahoochee.xlsx
+++ b/Dx_1998_Li_et_al_2_Paper02_Chattahoochee.xlsx
@@ -5444,7 +5444,7 @@
   <dimension ref="A1:X91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5692,7 +5692,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="45">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -5722,7 +5722,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="66">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -8099,11 +8099,11 @@
       </c>
       <c r="AB2" s="77">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>347</v>
+        <v>2173</v>
       </c>
       <c r="AC2" s="77">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>1066.6666666666667</v>
+        <v>3200</v>
       </c>
       <c r="AD2" s="77">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
@@ -8111,7 +8111,7 @@
       </c>
       <c r="AE2" s="75">
         <f t="shared" ref="AE2:AE3" si="0">Delta_T__seconds</f>
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="AF2" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8131,7 +8131,7 @@
       </c>
       <c r="AJ2" s="75">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>2556.4499999999998</v>
+        <v>852.14999999999986</v>
       </c>
       <c r="AK2" s="75">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -8149,7 +8149,7 @@
       </c>
       <c r="AO2" s="79">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>1066</v>
+        <v>3200</v>
       </c>
       <c r="AP2" s="79">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -8238,19 +8238,19 @@
       </c>
       <c r="AB3" s="77">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>581</v>
+        <v>3636</v>
       </c>
       <c r="AC3" s="77">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>1860</v>
+        <v>5580</v>
       </c>
       <c r="AD3" s="77">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>1066.6666666666667</v>
+        <v>3200</v>
       </c>
       <c r="AE3" s="75">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="AF3" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8270,7 +8270,7 @@
       </c>
       <c r="AJ3" s="75">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>2862.2999999999997</v>
+        <v>954.09999999999991</v>
       </c>
       <c r="AK3" s="75">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -8288,7 +8288,7 @@
       </c>
       <c r="AO3" s="79">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>1860</v>
+        <v>5580</v>
       </c>
       <c r="AP3" s="79">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -8377,19 +8377,19 @@
       </c>
       <c r="AB4" s="83">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>743</v>
+        <v>4648</v>
       </c>
       <c r="AC4" s="83">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>2433.3333333333335</v>
+        <v>7300</v>
       </c>
       <c r="AD4" s="83">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>1860</v>
+        <v>5580</v>
       </c>
       <c r="AE4" s="75">
         <f>Delta_T__seconds</f>
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="AF4" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8409,7 +8409,7 @@
       </c>
       <c r="AJ4" s="82">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>2556.4499999999998</v>
+        <v>852.14999999999986</v>
       </c>
       <c r="AK4" s="82">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -8423,7 +8423,7 @@
       <c r="AN4" s="75"/>
       <c r="AO4" s="79">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>2433</v>
+        <v>7300</v>
       </c>
       <c r="AP4" s="79">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -8512,19 +8512,19 @@
       </c>
       <c r="AB5" s="83">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>1065</v>
+        <v>6660</v>
       </c>
       <c r="AC5" s="83">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>3306.6666666666665</v>
+        <v>9920</v>
       </c>
       <c r="AD5" s="83">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>2433.3333333333335</v>
+        <v>7300</v>
       </c>
       <c r="AE5" s="75">
         <f>Delta_T__seconds</f>
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="AF5" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8544,7 +8544,7 @@
       </c>
       <c r="AJ5" s="82">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>2680.6499999999996</v>
+        <v>893.55</v>
       </c>
       <c r="AK5" s="82">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -8558,7 +8558,7 @@
       <c r="AN5" s="75"/>
       <c r="AO5" s="79">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>3306</v>
+        <v>9920</v>
       </c>
       <c r="AP5" s="79">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -8647,19 +8647,19 @@
       </c>
       <c r="AB6" s="83">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>1427</v>
+        <v>8923</v>
       </c>
       <c r="AC6" s="83">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>3806.6666666666665</v>
+        <v>11420</v>
       </c>
       <c r="AD6" s="83">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>3306.6666666666665</v>
+        <v>9920</v>
       </c>
       <c r="AE6" s="75">
         <f>Delta_T__seconds</f>
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="AF6" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8679,7 +8679,7 @@
       </c>
       <c r="AJ6" s="82">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>3049.2</v>
+        <v>1016.4</v>
       </c>
       <c r="AK6" s="82">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -8693,7 +8693,7 @@
       <c r="AN6" s="75"/>
       <c r="AO6" s="79">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>3806</v>
+        <v>11420</v>
       </c>
       <c r="AP6" s="79">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -8782,19 +8782,19 @@
       </c>
       <c r="AB7" s="83">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>1548</v>
+        <v>9675</v>
       </c>
       <c r="AC7" s="83">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>4033.3333333333335</v>
+        <v>12100</v>
       </c>
       <c r="AD7" s="83">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>3806.6666666666665</v>
+        <v>11420</v>
       </c>
       <c r="AE7" s="75">
         <f>Delta_T__seconds</f>
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="AF7" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8814,7 +8814,7 @@
       </c>
       <c r="AJ7" s="82">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>3049.2</v>
+        <v>1016.4</v>
       </c>
       <c r="AK7" s="82">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -8828,7 +8828,7 @@
       <c r="AN7" s="75"/>
       <c r="AO7" s="79">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>4033</v>
+        <v>12100</v>
       </c>
       <c r="AP7" s="79">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -8917,19 +8917,19 @@
       </c>
       <c r="AB8" s="83">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>2075</v>
+        <v>12969</v>
       </c>
       <c r="AC8" s="83">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>5106.666666666667</v>
+        <v>15320</v>
       </c>
       <c r="AD8" s="83">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>4033.3333333333335</v>
+        <v>12100</v>
       </c>
       <c r="AE8" s="75">
         <f>Delta_T__seconds</f>
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="AF8" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8949,7 +8949,7 @@
       </c>
       <c r="AJ8" s="82">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>2268</v>
+        <v>756</v>
       </c>
       <c r="AK8" s="82">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -8963,7 +8963,7 @@
       <c r="AN8" s="75"/>
       <c r="AO8" s="79">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>5106</v>
+        <v>15320</v>
       </c>
       <c r="AP8" s="79">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>

</xml_diff>